<commit_message>
Semana 2,3 y 4
</commit_message>
<xml_diff>
--- a/Documents/Tarea_2.xlsx
+++ b/Documents/Tarea_2.xlsx
@@ -8,27 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B99F21C7-127E-44FF-AABB-5AF4F271A61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0940D95D-EBA8-446C-B5EF-2B51218448D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Semana 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Semana 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Semana 3" sheetId="3" r:id="rId2"/>
+    <sheet name="Semana 2" sheetId="2" r:id="rId3"/>
     <sheet name="Semana 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Semana 1'!$A$1:$G$52</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Semana 2'!$A$1:$J$58</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Semana 3'!$A$1:$J$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Semana 2'!$A$1:$J$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Semana 3'!$A$1:$J$58</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="32">
   <si>
     <t>07:00 AM a 08:00 AM</t>
   </si>
@@ -122,6 +122,9 @@
   <si>
     <t>DOMINGO 19/02</t>
   </si>
+  <si>
+    <t>Lectura</t>
+  </si>
 </sst>
 </file>
 
@@ -524,32 +527,29 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -560,8 +560,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,19 +982,19 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="23" t="s">
         <v>17</v>
       </c>
       <c r="H5" s="4"/>
@@ -1001,11 +1004,11 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="3"/>
       <c r="I6" s="18"/>
     </row>
@@ -1016,16 +1019,16 @@
       <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="23" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="23" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="4"/>
@@ -1036,10 +1039,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="25"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="25"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="3"/>
       <c r="I8" s="18"/>
     </row>
@@ -1048,12 +1051,12 @@
         <v>5</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="26" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="23" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="23" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="4"/>
@@ -1069,11 +1072,11 @@
       <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="3"/>
       <c r="I10" s="18"/>
     </row>
@@ -1081,14 +1084,14 @@
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="25" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="21" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -1101,17 +1104,17 @@
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="21" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="24"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="31" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1120,22 +1123,22 @@
         <v>8</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="26" t="s">
+      <c r="D13" s="22"/>
+      <c r="E13" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="28"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="25"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="4"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
@@ -1150,10 +1153,10 @@
       <c r="E15" s="8"/>
       <c r="F15" s="3"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="31" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1166,26 +1169,26 @@
       <c r="E16" s="7"/>
       <c r="F16" s="4"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="28"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="23" t="s">
         <v>20</v>
       </c>
       <c r="H17" s="3"/>
@@ -1195,11 +1198,11 @@
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
       <c r="H18" s="5"/>
       <c r="I18" s="19"/>
     </row>
@@ -1238,26 +1241,656 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="32"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="32"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1265,12 +1898,327 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291E5A16-8BB5-4545-9E7B-DD444EE199AD}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="32"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>